<commit_message>
Updated results for full manual investigations
</commit_message>
<xml_diff>
--- a/results/differences_between_new-old_ok.xlsx
+++ b/results/differences_between_new-old_ok.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="20" yWindow="460" windowWidth="51200" windowHeight="26980" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="13940" windowWidth="51200" windowHeight="13500" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="differences_between_new-old_ok" sheetId="1" r:id="rId1"/>
@@ -1108,7 +1108,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P192"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="P28" sqref="P28"/>
     </sheetView>
   </sheetViews>

</xml_diff>